<commit_message>
Protein quantities in ng per ml
</commit_message>
<xml_diff>
--- a/inst/app/www/protein_quantitation_example.xlsx
+++ b/inst/app/www/protein_quantitation_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgijze\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgijze\Desktop\GlycoDash\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5C2537-4E72-4EC7-BD62-4A26E1816C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB944E-4CD0-43A1-B599-EC4A9158E5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25200" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>IgGI</t>
   </si>
@@ -48,9 +48,6 @@
     <t>labeled</t>
   </si>
   <si>
-    <t>standard_quantity</t>
-  </si>
-  <si>
     <t>IgG1</t>
   </si>
   <si>
@@ -61,6 +58,12 @@
   </si>
   <si>
     <t>IgGIVsil</t>
+  </si>
+  <si>
+    <t>standard_ ng</t>
+  </si>
+  <si>
+    <t>sample_ul</t>
   </si>
 </sst>
 </file>
@@ -392,11 +395,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -404,9 +405,10 @@
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -417,12 +419,15 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -433,10 +438,13 @@
       <c r="D2" s="2">
         <v>3</v>
       </c>
+      <c r="E2" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -447,19 +455,25 @@
       <c r="D3" s="2">
         <v>3</v>
       </c>
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix column name in quantitation example file
</commit_message>
<xml_diff>
--- a/inst/app/www/protein_quantitation_example.xlsx
+++ b/inst/app/www/protein_quantitation_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgijze\Desktop\GlycoDash\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB944E-4CD0-43A1-B599-EC4A9158E5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC938E26-D618-4756-B8BC-C7E9C020AE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25200" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,10 +60,10 @@
     <t>IgGIVsil</t>
   </si>
   <si>
-    <t>standard_ ng</t>
-  </si>
-  <si>
     <t>sample_ul</t>
+  </si>
+  <si>
+    <t>standard_ng</t>
   </si>
 </sst>
 </file>
@@ -419,10 +419,10 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>